<commit_message>
Projeto de busca no excel testado
</commit_message>
<xml_diff>
--- a/dados atuais.xlsx
+++ b/dados atuais.xlsx
@@ -4,20 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740" tabRatio="638" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7740" tabRatio="638" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dependentes" sheetId="2" r:id="rId1"/>
     <sheet name="planilha principal" sheetId="1" r:id="rId2"/>
     <sheet name="Completa" sheetId="17" r:id="rId3"/>
-    <sheet name="Validacao_Filtro" sheetId="18" r:id="rId4"/>
+    <sheet name="Base" sheetId="19" r:id="rId4"/>
+    <sheet name="validacao_filtro" sheetId="18" r:id="rId5"/>
+    <sheet name="Plan1" sheetId="20" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="capitulo_descricoes">#REF!</definedName>
+    <definedName name="capitulo_descricoes">Base!$F$3:$F$5</definedName>
     <definedName name="capitulos_ids">#REF!</definedName>
+    <definedName name="categorias">Base!$D$2:$D$9</definedName>
+    <definedName name="CG">Base!$A$2:$A$7</definedName>
     <definedName name="cidades">Completa!$B$2:$B$6</definedName>
-    <definedName name="grupo_descricoes">#REF!</definedName>
-    <definedName name="relacionamento">#REF!</definedName>
+    <definedName name="GC">Base!$C$2:$C$9</definedName>
+    <definedName name="grupo_descricoes">Base!$B$2:$B$7</definedName>
+    <definedName name="grupos">Base!$G$2:$G$4</definedName>
     <definedName name="SG">Completa!$A$2:$A$6</definedName>
     <definedName name="siglas">Completa!$F$2:$F$4</definedName>
   </definedNames>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="197">
   <si>
     <t>NOME</t>
   </si>
@@ -208,12 +213,6 @@
     <t>órtese pernas</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
     <t>ATENDIMENTO QUE NECESSITA</t>
   </si>
   <si>
@@ -299,6 +298,330 @@
   </si>
   <si>
     <t>Foz do Iguaçu</t>
+  </si>
+  <si>
+    <t>CAPITULO</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>GRUPO</t>
+  </si>
+  <si>
+    <t>'C00','C97','Neoplasias [tumores] malignas(os)');</t>
+  </si>
+  <si>
+    <t>C00','C75','Neoplasias [tumores] malignas(os)'</t>
+  </si>
+  <si>
+    <t>C00','C14','Neoplasias malignas do lábio'</t>
+  </si>
+  <si>
+    <t>Descrições</t>
+  </si>
+  <si>
+    <t>A00','B99','I - Algumas doenças infecciosas e parasitárias'</t>
+  </si>
+  <si>
+    <t>C00','D48','II - Neoplasias [tumores]'</t>
+  </si>
+  <si>
+    <t>D50','D89','III  - Doenças do sangue e dos órgãos hematopoéticos e alguns transtornos imunitários'</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>'A00','A09','Doenças infecciosas intestinais'</t>
+  </si>
+  <si>
+    <t>A06','Amebíase'</t>
+  </si>
+  <si>
+    <t>A07','Outras doenças intestinais por protozoários'</t>
+  </si>
+  <si>
+    <t>A08','Infecções intestinais virais'</t>
+  </si>
+  <si>
+    <t>'A15','A19','Tuberculose'</t>
+  </si>
+  <si>
+    <t>A15','Tuberculose respiratória'</t>
+  </si>
+  <si>
+    <t>A16','Tuberculose das vias respiratórias'</t>
+  </si>
+  <si>
+    <t>A17','Tuberculose do sistema nervoso'</t>
+  </si>
+  <si>
+    <t>A18','Tuberculose de outros órgãos'</t>
+  </si>
+  <si>
+    <t>A19','Tuberculose miliar'</t>
+  </si>
+  <si>
+    <t>'A20','A28','Algumas doenças bacterianas zoonóticas'</t>
+  </si>
+  <si>
+    <t>A00','A09','Doenças infecciosas intestinais'</t>
+  </si>
+  <si>
+    <t>A15','A19','Tuberculose'</t>
+  </si>
+  <si>
+    <t>A20','A28','Algumas doenças bacterianas zoonóticas'</t>
+  </si>
+  <si>
+    <t>A00</t>
+  </si>
+  <si>
+    <t>B99</t>
+  </si>
+  <si>
+    <t>I - Algumas doenças infecciosas e parasitárias</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>Doenças infecciosas intestinais</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>Tuberculose</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>Algumas doenças bacterianas zoonóticas</t>
+  </si>
+  <si>
+    <t>A30</t>
+  </si>
+  <si>
+    <t>A49</t>
+  </si>
+  <si>
+    <t>Outras doenças bacterianas</t>
+  </si>
+  <si>
+    <t>A50</t>
+  </si>
+  <si>
+    <t>A64</t>
+  </si>
+  <si>
+    <t>Infecções de transmissão predominantemente sexual</t>
+  </si>
+  <si>
+    <t>A65</t>
+  </si>
+  <si>
+    <t>A69</t>
+  </si>
+  <si>
+    <t>Outras doenças por espiroquetas</t>
+  </si>
+  <si>
+    <t>A70</t>
+  </si>
+  <si>
+    <t>A74</t>
+  </si>
+  <si>
+    <t>Outras doenças causadas por clamídias</t>
+  </si>
+  <si>
+    <t>A75</t>
+  </si>
+  <si>
+    <t>A79</t>
+  </si>
+  <si>
+    <t>Rickettsioses</t>
+  </si>
+  <si>
+    <t>A80</t>
+  </si>
+  <si>
+    <t>A89</t>
+  </si>
+  <si>
+    <t>Infecções virais do sistema nervoso central</t>
+  </si>
+  <si>
+    <t>A90</t>
+  </si>
+  <si>
+    <t>A99</t>
+  </si>
+  <si>
+    <t>Febres por arbovírus e febres hemorrágicas virais</t>
+  </si>
+  <si>
+    <t>B00</t>
+  </si>
+  <si>
+    <t>B09</t>
+  </si>
+  <si>
+    <t>Infecções virais caracterizadas por lesões de pele...</t>
+  </si>
+  <si>
+    <t>B15</t>
+  </si>
+  <si>
+    <t>B19</t>
+  </si>
+  <si>
+    <t>Hepatite viral</t>
+  </si>
+  <si>
+    <t>B20</t>
+  </si>
+  <si>
+    <t>B24</t>
+  </si>
+  <si>
+    <t>Doença pelo vírus da imunodeficiência humana [HIV]</t>
+  </si>
+  <si>
+    <t>B25</t>
+  </si>
+  <si>
+    <t>B34</t>
+  </si>
+  <si>
+    <t>Outras doenças por vírus</t>
+  </si>
+  <si>
+    <t>B35</t>
+  </si>
+  <si>
+    <t>B49</t>
+  </si>
+  <si>
+    <t>Micoses</t>
+  </si>
+  <si>
+    <t>B50</t>
+  </si>
+  <si>
+    <t>B64</t>
+  </si>
+  <si>
+    <t>Doenças devidas a protozoários</t>
+  </si>
+  <si>
+    <t>B65</t>
+  </si>
+  <si>
+    <t>B83</t>
+  </si>
+  <si>
+    <t>Helmintíases</t>
+  </si>
+  <si>
+    <t>B85</t>
+  </si>
+  <si>
+    <t>B89</t>
+  </si>
+  <si>
+    <t>Pediculose</t>
+  </si>
+  <si>
+    <t>B90</t>
+  </si>
+  <si>
+    <t>B94</t>
+  </si>
+  <si>
+    <t>Seqüelas de doenças infecciosas e parasitárias</t>
+  </si>
+  <si>
+    <t>B95</t>
+  </si>
+  <si>
+    <t>B97</t>
+  </si>
+  <si>
+    <t>Agentes de infecções bacterianas</t>
+  </si>
+  <si>
+    <t>Outras doenças infecciosas</t>
+  </si>
+  <si>
+    <t>C00</t>
+  </si>
+  <si>
+    <t>D48</t>
+  </si>
+  <si>
+    <t>II - Neoplasias [tumores]</t>
+  </si>
+  <si>
+    <t>C97</t>
+  </si>
+  <si>
+    <t>Neoplasias [tumores] malignas(os)</t>
+  </si>
+  <si>
+    <t>C75</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>Neoplasias malignas do lábio</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>Neoplasias malignas dos órgãos digestivos</t>
+  </si>
+  <si>
+    <t>C30</t>
+  </si>
+  <si>
+    <t>C39</t>
+  </si>
+  <si>
+    <t>Neoplasias malignas do aparelho respiratório e dos...</t>
+  </si>
+  <si>
+    <t>A00 B99 I - Algumas doenças infecciosas e parasitárias</t>
+  </si>
+  <si>
+    <t>C00 D48 II - Neoplasias [tumores]</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Aquira</t>
   </si>
 </sst>
 </file>
@@ -308,7 +631,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,8 +767,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,6 +966,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFDFDF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -801,7 +1148,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -838,6 +1185,20 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1181,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,48 +1566,122 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="22" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="22" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" s="22" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1257,13 +1692,13 @@
           <x14:formula1>
             <xm:f>'planilha principal'!$A$13:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C15</xm:sqref>
+          <xm:sqref>C2:C17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Nome não permitido. É preciso escolher uma das pessoas cadastradas na planilha principal. Por favor, clique em cancelar e escolha uma pessoa">
           <x14:formula1>
             <xm:f>'planilha principal'!$C$4:$C$362</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A14</xm:sqref>
+          <xm:sqref>A2:A16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1275,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI196"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
@@ -1309,25 +1744,25 @@
   <sheetData>
     <row r="1" spans="1:35" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B1" s="14"/>
       <c r="R1" s="9" t="s">
         <v>29</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AD1" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AF1" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
@@ -1393,7 +1828,7 @@
         <v>49</v>
       </c>
       <c r="W2" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="X2" s="16" t="s">
         <v>18</v>
@@ -1408,22 +1843,22 @@
         <v>51</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AF2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AG2" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH2" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="AI2" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:35" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1472,16 +1907,16 @@
       </c>
       <c r="O4" s="8"/>
       <c r="W4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="AC4" t="s">
         <v>54</v>
       </c>
       <c r="AE4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AI4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -1498,10 +1933,10 @@
         <v>16</v>
       </c>
       <c r="AC5" t="s">
-        <v>60</v>
+        <v>193</v>
       </c>
       <c r="AE5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -1515,7 +1950,7 @@
         <v>17</v>
       </c>
       <c r="AC6" t="s">
-        <v>61</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -1684,7 +2119,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B29" s="2">
         <v>26</v>
@@ -1692,7 +2127,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B30" s="2">
         <v>27</v>
@@ -1700,7 +2135,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B31" s="2">
         <v>28</v>
@@ -1713,7 +2148,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" s="2">
         <v>30</v>
@@ -1721,7 +2156,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="2">
         <v>31</v>
@@ -2590,62 +3025,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
         <v>85</v>
-      </c>
-      <c r="F4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2655,44 +3090,254 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="6" max="6" width="89.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
         <v>82</v>
       </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A5">
       <formula1>siglas</formula1>
     </dataValidation>
@@ -2702,13 +3347,573 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3">
       <formula1>OFFSET(cidades,MATCH(A2,SG,0)-1,0,COUNTIF(SG,A2))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D5">
       <formula1>capitulo_descricoes</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:F5">
+      <formula1>OFFSET(grupo_descricoes,MATCH(#REF!,CG,0)-1,0,COUNTIF(CG,#REF!))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4">
+      <formula1>OFFSET(grupo_descricoes,MATCH(D3,CG,0)-1,0,COUNTIF(CG,D3))</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
-      <formula1>OFFSET(grupo_descricoes,MATCH(E2,relacionamento,0)-1,0,COUNTIF(relacionamento,E2))</formula1>
+      <formula1>grupos</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
+      <formula1>OFFSET(categorias,MATCH(F2,GC,0)-1,0,COUNTIF(GC,F2))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="52.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>